<commit_message>
ntah darimana inii :(
</commit_message>
<xml_diff>
--- a/test/run_results.xlsx
+++ b/test/run_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\.juliapro\JuliaPro_v1.4.2-1\dev\Tomato\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F809E820-62E7-4B58-AD28-BDA2229949FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16774B15-D091-4D8F-A8E8-2F5E3A5B3348}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="2655" windowWidth="20490" windowHeight="10920" xr2:uid="{421E56CE-D904-4426-B536-95ECBDBA6057}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{421E56CE-D904-4426-B536-95ECBDBA6057}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -281,17 +281,17 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B474372F-4FD3-4AFA-B4A8-BF7FC79460CA}">
   <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,155 +620,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="4">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4">
         <v>2</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4">
         <v>4</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4">
         <v>5</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4">
         <v>6</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4">
         <v>7</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3">
+      <c r="S1" s="4"/>
+      <c r="T1" s="4">
         <v>8</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3">
+      <c r="U1" s="4"/>
+      <c r="V1" s="4">
         <v>9</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4">
         <v>10</v>
       </c>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3">
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4">
         <v>11</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4">
         <v>12</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4">
         <v>13</v>
       </c>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3">
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4">
         <v>14</v>
       </c>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3">
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4">
         <v>15</v>
       </c>
-      <c r="AI1" s="3"/>
+      <c r="AI1" s="4"/>
     </row>
     <row r="2" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2" t="s">
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2" t="s">
+      <c r="W2" s="3"/>
+      <c r="X2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2" t="s">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2" t="s">
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2" t="s">
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2" t="s">
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2" t="s">
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="2"/>
+      <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" t="s">
         <v>1</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="Q12">
         <v>0.183</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="2">
         <v>2115.2440000000001</v>
       </c>
       <c r="S12">
@@ -1551,7 +1551,7 @@
       <c r="Q13">
         <v>31.35</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="2">
         <v>3637.4740000000002</v>
       </c>
       <c r="S13">
@@ -1622,7 +1622,7 @@
       <c r="Q14">
         <v>31.905000000000001</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="2">
         <v>7908.4880000000003</v>
       </c>
       <c r="S14">
@@ -1693,7 +1693,7 @@
       <c r="Q15">
         <v>0.184</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="2">
         <v>2115.2440000000001</v>
       </c>
       <c r="S15">
@@ -1731,7 +1731,7 @@
       <c r="F16">
         <v>2299.8449999999998</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="1">
         <v>41536</v>
       </c>
       <c r="H16">
@@ -2375,13 +2375,18 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
@@ -2398,18 +2403,13 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>